<commit_message>
Taxid noexist파일 점검 시작
</commit_message>
<xml_diff>
--- a/KS_Invoice 추출 및 정리_통합본/Data/Config.xlsx
+++ b/KS_Invoice 추출 및 정리_통합본/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\KS_Invoice 추출 및 정리_통합본\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkh08\OneDrive\문서\uipath\alphaco5_teamproject2\alphaco5_teamproejct2\KS_Invoice 추출 및 정리_통합본\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C0BDB0-190F-4BC5-AC83-C27FF23E5C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E53A86F-9E2B-407D-864D-5436ACD1F42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{46CAC932-19BF-4421-AA43-1A3B90B5C468}"/>
+    <workbookView xWindow="3930" yWindow="3930" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{46CAC932-19BF-4421-AA43-1A3B90B5C468}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>제목</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -827,6 +827,95 @@
   </si>
   <si>
     <t>AddInvoice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISO_Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C:\RPA\KS_Invoice </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>추출</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정리</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>통합본</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>\Template\ISO_MasterTable.xlsx</t>
+    </r>
+  </si>
+  <si>
+    <t>ISO_Code_Exel_Path</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -834,7 +923,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -901,6 +990,13 @@
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="돋움"/>
+      <family val="3"/>
       <charset val="129"/>
     </font>
   </fonts>
@@ -1323,16 +1419,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D129B3-C630-4D4F-94AA-81D79A80C13C}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.75" style="1" customWidth="1"/>
-    <col min="2" max="3" width="40.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="63.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.75" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
@@ -1411,6 +1508,17 @@
       </c>
       <c r="C7" s="1" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>